<commit_message>
trying parameters for excess return calculation
</commit_message>
<xml_diff>
--- a/temp/SYWG pri.xlsx
+++ b/temp/SYWG pri.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>证券代码</t>
   </si>
@@ -32,11 +32,6 @@
     <t>证券简称</t>
   </si>
   <si>
-    <t>总市值2_x000D_
-[交易日期] 最新收盘日_x000D_
-[单位] 元</t>
-  </si>
-  <si>
     <t>801010.SI</t>
   </si>
   <si>
@@ -203,29 +198,16 @@
   </si>
   <si>
     <t>机械设备(申万)</t>
-  </si>
-  <si>
-    <t>数据来源：Wind资讯</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="###,###,###,##0.0000"/>
-  </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -266,27 +248,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -603,343 +573,251 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L6" sqref="L6"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.88671875" style="1"/>
-    <col min="3" max="3" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="19.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="6" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="7">
-        <v>966578831095.99902</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="6" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="7">
-        <v>2192271695550</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="6" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="7">
-        <v>2817449217164</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="6" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="7">
-        <v>578824714450</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="6" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="7">
-        <v>1482916020918</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="6" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="7">
-        <v>1923384114314</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="6" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="7">
-        <v>962884368610</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+      <c r="B9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="6" t="s">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="7">
-        <v>1637709999432</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="6" t="s">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="7">
-        <v>687326727468</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="B11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="6" t="s">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="7">
-        <v>826436870307</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="B12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="6" t="s">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="7">
-        <v>3102414838228</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+      <c r="B13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="6" t="s">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="7">
-        <v>1982023051969</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+      <c r="B14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="6" t="s">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="7">
-        <v>1610570578488</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
+      <c r="B15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="6" t="s">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="7">
-        <v>2273425810749</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
+      <c r="B16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="6" t="s">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="7">
-        <v>987722482080</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
+      <c r="B17" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="6" t="s">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="7">
-        <v>370480425842.99902</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
+      <c r="B18" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="6" t="s">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="7">
-        <v>362344136514</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
+      <c r="B19" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="6" t="s">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="7">
-        <v>558033708413</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
+      <c r="B20" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="6" t="s">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="7">
-        <v>1482130211615</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
+      <c r="B21" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="6" t="s">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="7">
-        <v>1694562534538</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
+      <c r="B22" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="6" t="s">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="7">
-        <v>767160986940</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="6" t="s">
+      <c r="B23" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="6" t="s">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="7">
-        <v>2232497033097</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="6" t="s">
+      <c r="B24" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="6" t="s">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="7">
-        <v>1957482450449</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="6" t="s">
+      <c r="B25" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="6" t="s">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="7">
-        <v>902551724977</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="6" t="s">
+      <c r="B26" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="6" t="s">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="7">
-        <v>5205179137821</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="6" t="s">
+      <c r="B27" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B27" s="6" t="s">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="7">
-        <v>3179461493144</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="6" t="s">
+      <c r="B28" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="6" t="s">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="7">
-        <v>1918191261731</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="6" t="s">
+      <c r="B29" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="7">
-        <v>2287333740723</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>